<commit_message>
working application and JUnit tests
</commit_message>
<xml_diff>
--- a/documentation/Assignment1-ERD.xlsx
+++ b/documentation/Assignment1-ERD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SangivGiovanni\Desktop\Assignment1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SangivGiovanni\Desktop\IMS-Starter\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF5F59F-22DF-4C0C-A9EB-0CDA329FA637}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933E370C-9C66-4AFB-A716-FB0EFCFB0C61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{493BD57B-97CE-48FF-B816-388D840320F1}"/>
   </bookViews>
@@ -250,6 +250,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -259,7 +260,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,7 +577,7 @@
   <dimension ref="D5:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,21 +593,21 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="H5" s="11" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="H5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="L5" s="12" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="L5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D6" s="4" t="s">
@@ -648,7 +648,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>15</v>
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
@@ -702,9 +702,9 @@
       </c>
     </row>
     <row r="9" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
         <v>12</v>
@@ -721,9 +721,9 @@
       </c>
     </row>
     <row r="10" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="14" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D14" t="s">

</xml_diff>